<commit_message>
Change Exposures class: it is a GeoDataFrame now.
</commit_message>
<xml_diff>
--- a/climada/engine/test/data/demo_future_TEST.xlsx
+++ b/climada/engine/test/data/demo_future_TEST.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aznarsig/Documents/Python/climada_python/climada/engine/test/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BAA3B260-07EF-3848-A5AF-5057D8E8B8A9}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="15140" windowHeight="13060" tabRatio="766"/>
+    <workbookView xWindow="11320" yWindow="4940" windowWidth="15140" windowHeight="13060" tabRatio="766" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="assets" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
     <sheet name="_measures_details" sheetId="5" r:id="rId6"/>
     <sheet name="_discounting_sheet" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,13 +31,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>srzdnb</author>
     <author>A satisfied Microsoft Office user</author>
   </authors>
   <commentList>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -98,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -165,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -234,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="1">
+    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
       <text>
         <r>
           <rPr>
@@ -246,7 +252,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="0">
+    <comment ref="A14" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
       <text>
         <r>
           <rPr>
@@ -259,7 +265,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A23" authorId="0">
+    <comment ref="A23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
       <text>
         <r>
           <rPr>
@@ -277,14 +283,14 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>srzdnb</author>
     <author>David Bresch</author>
     <author>sarah</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -297,7 +303,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -310,7 +316,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -323,7 +329,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -338,7 +344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -352,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="1">
+    <comment ref="F1" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -365,7 +371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -452,7 +458,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -539,7 +545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
@@ -626,7 +632,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -713,7 +719,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -732,7 +738,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="2">
+    <comment ref="L1" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -746,7 +752,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="2">
+    <comment ref="M1" authorId="2" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -765,27 +771,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="76">
   <si>
     <t>Intensity</t>
   </si>
   <si>
     <t>MDD</t>
-  </si>
-  <si>
-    <t>Deductible</t>
-  </si>
-  <si>
-    <t>Cover</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>Value</t>
   </si>
   <si>
     <t>MDR</t>
@@ -991,11 +982,29 @@
   <si>
     <t>TC</t>
   </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>deductible</t>
+  </si>
+  <si>
+    <t>cover</t>
+  </si>
+  <si>
+    <t>if_TC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1172,7 +1181,7 @@
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1245,11 +1254,19 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1289,7 +1306,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.399185252705481"/>
-          <c:y val="0.0387596262005711"/>
+          <c:y val="3.87596262005711E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1308,9 +1325,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.107942973523422"/>
-          <c:y val="0.240310987126738"/>
-          <c:w val="0.830957230142566"/>
-          <c:h val="0.465118039600138"/>
+          <c:y val="0.24031098712673801"/>
+          <c:w val="0.83095723014256595"/>
+          <c:h val="0.46511803960013798"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1360,40 +1377,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90.0</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110.0</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1405,7 +1422,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.01</c:v>
@@ -1444,6 +1461,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C2D4-294F-9F0C-C9F06B05B5DE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1489,40 +1511,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90.0</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110.0</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1534,7 +1556,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.01</c:v>
@@ -1543,22 +1565,22 @@
                   <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.057</c:v>
+                  <c:v>5.6999999999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.14</c:v>
+                  <c:v>0.14000000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.177</c:v>
+                  <c:v>0.17700000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.214</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.28</c:v>
+                  <c:v>0.28000000000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.34</c:v>
@@ -1573,6 +1595,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C2D4-294F-9F0C-C9F06B05B5DE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1618,40 +1645,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10.0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>90.0</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>110.0</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1663,34 +1690,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0001</c:v>
+                  <c:v>1E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0002</c:v>
+                  <c:v>2.0000000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.00171</c:v>
+                  <c:v>1.7099999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.01</c:v>
+                  <c:v>1.0000000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.021</c:v>
+                  <c:v>2.1000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0354</c:v>
+                  <c:v>3.5400000000000008E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0642</c:v>
+                  <c:v>6.4199999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.112</c:v>
+                  <c:v>0.11200000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.153</c:v>
+                  <c:v>0.15300000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.2</c:v>
@@ -1702,6 +1729,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-C2D4-294F-9F0C-C9F06B05B5DE}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1758,8 +1790,8 @@
         <c:axId val="2099068824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
-          <c:min val="0.0"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1819,9 +1851,9 @@
           <c:wMode val="edge"/>
           <c:hMode val="edge"/>
           <c:x val="0.320197432217524"/>
-          <c:y val="0.873624643073462"/>
-          <c:w val="0.716749544238005"/>
-          <c:h val="0.972525741974561"/>
+          <c:y val="0.87362464307346199"/>
+          <c:w val="0.71674954423800497"/>
+          <c:h val="0.97252574197456099"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1883,14 +1915,14 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1929,8 +1961,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.399185319893981"/>
-          <c:y val="0.0387596262005711"/>
+          <c:x val="0.39918531989398098"/>
+          <c:y val="3.87596262005711E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1949,9 +1981,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.107942973523422"/>
-          <c:y val="0.240310987126738"/>
-          <c:w val="0.830957230142566"/>
-          <c:h val="0.465118039600138"/>
+          <c:y val="0.24031098712673801"/>
+          <c:w val="0.83095723014256595"/>
+          <c:h val="0.46511803960013798"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2001,31 +2033,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2037,36 +2069,41 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0218571428571429</c:v>
+                  <c:v>2.1857142857142856E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0358875</c:v>
+                  <c:v>3.5887499999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0539774153074028</c:v>
+                  <c:v>5.3977415307402764E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.103534246575342</c:v>
+                  <c:v>0.10353424657534246</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.180414</c:v>
+                  <c:v>0.18041399999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.410796</c:v>
+                  <c:v>0.41079599999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.410796</c:v>
+                  <c:v>0.41079599999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0575-1E49-91AB-2AF2F67A7151}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2112,31 +2149,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2148,36 +2185,41 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.005</c:v>
+                  <c:v>5.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.042</c:v>
+                  <c:v>4.2000000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.3985</c:v>
+                  <c:v>0.39850000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.657</c:v>
+                  <c:v>0.65700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0575-1E49-91AB-2AF2F67A7151}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2211,31 +2253,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2247,36 +2289,41 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.000918</c:v>
+                  <c:v>9.1799999999999998E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.005742</c:v>
+                  <c:v>5.7419999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.02151</c:v>
+                  <c:v>2.1510000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.068022</c:v>
+                  <c:v>6.8021999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.180414</c:v>
+                  <c:v>0.18041399999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.410796</c:v>
+                  <c:v>0.41079599999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.410796</c:v>
+                  <c:v>0.41079599999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0575-1E49-91AB-2AF2F67A7151}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2333,8 +2380,8 @@
         <c:axId val="2099158744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
-          <c:min val="0.0"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2393,10 +2440,10 @@
           <c:yMode val="edge"/>
           <c:wMode val="edge"/>
           <c:hMode val="edge"/>
-          <c:x val="0.321867128402561"/>
-          <c:y val="0.873624643073462"/>
-          <c:w val="0.717444137050436"/>
-          <c:h val="0.972525741974561"/>
+          <c:x val="0.32186712840256099"/>
+          <c:y val="0.87362464307346199"/>
+          <c:w val="0.71744413705043597"/>
+          <c:h val="0.97252574197456099"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2458,14 +2505,14 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2504,8 +2551,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.398374896012691"/>
-          <c:y val="0.0386102147067682"/>
+          <c:x val="0.39837489601269099"/>
+          <c:y val="3.8610214706768203E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2523,10 +2570,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.107723791054908"/>
+          <c:x val="0.10772379105490799"/>
           <c:y val="0.239382690679843"/>
-          <c:w val="0.831302463046365"/>
-          <c:h val="0.467182347939694"/>
+          <c:w val="0.83130246304636501"/>
+          <c:h val="0.46718234793969399"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -2576,31 +2623,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2612,25 +2659,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.025</c:v>
+                  <c:v>2.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.054054054054054</c:v>
+                  <c:v>5.4054054054054057E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.104615384615385</c:v>
+                  <c:v>0.10461538461538462</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.211764705882353</c:v>
+                  <c:v>0.21176470588235294</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.4</c:v>
@@ -2642,6 +2689,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9817-294B-96DB-6BA11909474C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2687,31 +2739,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2723,13 +2775,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.004</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.16</c:v>
@@ -2744,15 +2796,20 @@
                   <c:v>0.85</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9817-294B-96DB-6BA11909474C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2786,31 +2843,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30.0</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40.0</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.0</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>70.0</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80.0</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>100.0</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2822,22 +2879,22 @@
                 <c:formatCode>_(* #\'##0.000000_);_(* \(#\'##0.000000\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.004</c:v>
+                  <c:v>4.0000000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.068</c:v>
+                  <c:v>6.8000000000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.18</c:v>
@@ -2852,6 +2909,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9817-294B-96DB-6BA11909474C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2908,8 +2970,8 @@
         <c:axId val="2099205000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1.0"/>
-          <c:min val="0.0"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2968,10 +3030,10 @@
           <c:yMode val="edge"/>
           <c:wMode val="edge"/>
           <c:hMode val="edge"/>
-          <c:x val="0.324323937394803"/>
-          <c:y val="0.874316509616626"/>
-          <c:w val="0.719900946042678"/>
-          <c:h val="0.972677165354331"/>
+          <c:x val="0.32432393739480297"/>
+          <c:y val="0.87431650961662599"/>
+          <c:w val="0.71990094604267796"/>
+          <c:h val="0.97267716535433102"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3033,7 +3095,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3056,7 +3118,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1254" name="Chart 1"/>
+        <xdr:cNvPr id="1254" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000E6040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3088,7 +3156,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1255" name="Chart 4"/>
+        <xdr:cNvPr id="1255" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000E7040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3120,7 +3194,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="1256" name="Chart 9"/>
+        <xdr:cNvPr id="1256" name="Chart 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000E8040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3461,14 +3541,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" style="1" bestFit="1" customWidth="1"/>
@@ -3479,30 +3559,30 @@
     <col min="7" max="7" width="13.1640625" style="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>72</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>73</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>74</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>26.933899</v>
       </c>
@@ -3527,7 +3607,7 @@
         <v>5139300504.6792002</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>26.957203</v>
       </c>
@@ -3552,7 +3632,7 @@
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>26.783846</v>
       </c>
@@ -3577,7 +3657,7 @@
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>26.645524000000002</v>
       </c>
@@ -3602,7 +3682,7 @@
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>26.897796</v>
       </c>
@@ -3627,7 +3707,7 @@
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>26.925359</v>
       </c>
@@ -3652,7 +3732,7 @@
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>26.914767999999999</v>
       </c>
@@ -3677,7 +3757,7 @@
         <v>4648538819.2559605</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>26.853491000000002</v>
       </c>
@@ -3702,7 +3782,7 @@
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>26.845099000000001</v>
       </c>
@@ -3727,7 +3807,7 @@
         <v>4657184266.3798704</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>26.826509999999999</v>
       </c>
@@ -3752,7 +3832,7 @@
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>26.842772</v>
       </c>
@@ -3777,7 +3857,7 @@
         <v>4651025709.2825003</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>26.825904999999999</v>
       </c>
@@ -3802,7 +3882,7 @@
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>26.804649999999999</v>
       </c>
@@ -3827,7 +3907,7 @@
         <v>4961290391.9390001</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>26.788648999999999</v>
       </c>
@@ -3852,7 +3932,7 @@
         <v>5438960829.5693903</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>26.704277000000001</v>
       </c>
@@ -3877,7 +3957,7 @@
         <v>4651450127.7348204</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>26.710049999999999</v>
       </c>
@@ -3902,7 +3982,7 @@
         <v>4800322701.0994797</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>26.755412</v>
       </c>
@@ -3927,7 +4007,7 @@
         <v>4653832934.1885204</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>26.678449000000001</v>
       </c>
@@ -3952,7 +4032,7 @@
         <v>4661009648.1131401</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>26.725649000000001</v>
       </c>
@@ -3977,7 +4057,7 @@
         <v>4648800543.9682198</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>26.720599</v>
       </c>
@@ -4002,7 +4082,7 @@
         <v>4649451965.6613197</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>26.71255</v>
       </c>
@@ -4027,7 +4107,7 @@
         <v>4648559312.6040897</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>26.664899999999999</v>
       </c>
@@ -4052,7 +4132,7 @@
         <v>4728611180.8810101</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>26.664698999999999</v>
       </c>
@@ -4077,7 +4157,7 @@
         <v>4657477654.7297096</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>26.663149000000001</v>
       </c>
@@ -4102,7 +4182,7 @@
         <v>4648537081.1613503</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>26.668749999999999</v>
       </c>
@@ -4127,7 +4207,7 @@
         <v>4648940804.1615105</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>26.638517</v>
       </c>
@@ -4152,7 +4232,7 @@
         <v>4648357404.0137701</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>26.59309</v>
       </c>
@@ -4177,7 +4257,7 @@
         <v>4702738672.44872</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>26.617449000000001</v>
       </c>
@@ -4202,7 +4282,7 @@
         <v>4652378148.9963999</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>26.620079</v>
       </c>
@@ -4227,7 +4307,7 @@
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>26.596795</v>
       </c>
@@ -4252,7 +4332,7 @@
         <v>4681799806.2101603</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>26.577048999999999</v>
       </c>
@@ -4277,7 +4357,7 @@
         <v>4849820094.44631</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>26.524584999999998</v>
       </c>
@@ -4302,7 +4382,7 @@
         <v>4958704187.9946203</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>26.524158</v>
       </c>
@@ -4327,7 +4407,7 @@
         <v>4700541195.3858604</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>26.523737000000001</v>
       </c>
@@ -4352,7 +4432,7 @@
         <v>4648479198.5686197</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>26.520284</v>
       </c>
@@ -4377,7 +4457,7 @@
         <v>4693012294.9874296</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>26.547349000000001</v>
       </c>
@@ -4402,7 +4482,7 @@
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>26.463398999999999</v>
       </c>
@@ -4427,7 +4507,7 @@
         <v>4658942386.6735201</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>26.459050000000001</v>
       </c>
@@ -4452,7 +4532,7 @@
         <v>4648115411.3237801</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>26.455580000000001</v>
       </c>
@@ -4477,7 +4557,7 @@
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>26.453699</v>
       </c>
@@ -4502,7 +4582,7 @@
         <v>9034864234.9035301</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>26.449998999999998</v>
       </c>
@@ -4527,7 +4607,7 @@
         <v>4813012085.2491903</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>26.397299</v>
       </c>
@@ -4552,7 +4632,7 @@
         <v>4647994148.9088297</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>26.4084</v>
       </c>
@@ -4577,7 +4657,7 @@
         <v>6762158257.6236</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>26.408750000000001</v>
       </c>
@@ -4602,7 +4682,7 @@
         <v>4653572219.9963903</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>26.379113</v>
       </c>
@@ -4627,7 +4707,7 @@
         <v>5313371933.3403101</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>26.3809</v>
       </c>
@@ -4652,7 +4732,7 @@
         <v>4662182013.1408501</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>26.349067999999999</v>
       </c>
@@ -4677,7 +4757,7 @@
         <v>4666138563.2157402</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>26.346349</v>
       </c>
@@ -4702,7 +4782,7 @@
         <v>4728552813.2386103</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>26.348015</v>
       </c>
@@ -4727,7 +4807,7 @@
         <v>4650520449.2202196</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>26.347957000000001</v>
       </c>
@@ -4764,14 +4844,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:XFD65536"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
@@ -4781,9 +4861,9 @@
     <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -4792,16 +4872,16 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" s="5">
         <v>2</v>
       </c>
@@ -4819,10 +4899,10 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -4840,10 +4920,10 @@
         <v>1E-4</v>
       </c>
       <c r="F3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -4861,10 +4941,10 @@
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" s="5">
         <v>2</v>
       </c>
@@ -4882,10 +4962,10 @@
         <v>1.7099999999999997E-3</v>
       </c>
       <c r="F5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" s="5">
         <v>2</v>
       </c>
@@ -4903,10 +4983,10 @@
         <v>1.0000000000000002E-2</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" s="5">
         <v>2</v>
       </c>
@@ -4924,10 +5004,10 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="F7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="5">
         <v>2</v>
       </c>
@@ -4945,10 +5025,10 @@
         <v>3.5400000000000008E-2</v>
       </c>
       <c r="F8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="5">
         <v>2</v>
       </c>
@@ -4966,10 +5046,10 @@
         <v>6.4199999999999993E-2</v>
       </c>
       <c r="F9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" s="5">
         <v>2</v>
       </c>
@@ -4987,10 +5067,10 @@
         <v>0.11200000000000002</v>
       </c>
       <c r="F10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" s="5">
         <v>2</v>
       </c>
@@ -5008,10 +5088,10 @@
         <v>0.15300000000000002</v>
       </c>
       <c r="F11" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" s="5">
         <v>2</v>
       </c>
@@ -5029,10 +5109,10 @@
         <v>0.2</v>
       </c>
       <c r="F12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" s="5">
         <v>2</v>
       </c>
@@ -5050,10 +5130,10 @@
         <v>0.25</v>
       </c>
       <c r="F13" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" s="4">
         <v>1</v>
       </c>
@@ -5070,10 +5150,10 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" s="4">
         <v>1</v>
       </c>
@@ -5091,10 +5171,10 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" s="4">
         <v>1</v>
       </c>
@@ -5112,10 +5192,10 @@
         <v>9.1799999999999998E-4</v>
       </c>
       <c r="F16" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" s="4">
         <v>1</v>
       </c>
@@ -5133,10 +5213,10 @@
         <v>5.7419999999999997E-3</v>
       </c>
       <c r="F17" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" s="4">
         <v>1</v>
       </c>
@@ -5154,10 +5234,10 @@
         <v>2.1510000000000001E-2</v>
       </c>
       <c r="F18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>1</v>
       </c>
@@ -5175,10 +5255,10 @@
         <v>6.8021999999999999E-2</v>
       </c>
       <c r="F19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="4">
         <v>1</v>
       </c>
@@ -5196,10 +5276,10 @@
         <v>0.18041399999999999</v>
       </c>
       <c r="F20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="4">
         <v>1</v>
       </c>
@@ -5217,10 +5297,10 @@
         <v>0.41079599999999999</v>
       </c>
       <c r="F21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" s="4">
         <v>1</v>
       </c>
@@ -5238,10 +5318,10 @@
         <v>0.41079599999999999</v>
       </c>
       <c r="F22" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" s="4">
         <v>3</v>
       </c>
@@ -5258,10 +5338,10 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" s="4">
         <v>3</v>
       </c>
@@ -5279,10 +5359,10 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" s="4">
         <v>3</v>
       </c>
@@ -5299,10 +5379,10 @@
         <v>0</v>
       </c>
       <c r="F25" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" s="4">
         <v>3</v>
       </c>
@@ -5320,10 +5400,10 @@
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="F26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" s="4">
         <v>3</v>
       </c>
@@ -5341,10 +5421,10 @@
         <v>0.02</v>
       </c>
       <c r="F27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" s="4">
         <v>3</v>
       </c>
@@ -5362,10 +5442,10 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="F28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" s="4">
         <v>3</v>
       </c>
@@ -5383,10 +5463,10 @@
         <v>0.18</v>
       </c>
       <c r="F29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" s="4">
         <v>3</v>
       </c>
@@ -5404,10 +5484,10 @@
         <v>0.4</v>
       </c>
       <c r="F30" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" s="4">
         <v>3</v>
       </c>
@@ -5425,7 +5505,7 @@
         <v>0.4</v>
       </c>
       <c r="F31" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -5443,14 +5523,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
@@ -5464,53 +5544,53 @@
     <col min="13" max="13" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="M1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C2" s="8">
         <f>_measures_details!B12*3*3*2.1</f>
@@ -5523,7 +5603,7 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -5538,7 +5618,7 @@
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="L2">
         <v>0</v>
@@ -5547,12 +5627,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C3" s="11">
         <f>30000000*4*6*2.4</f>
@@ -5565,7 +5645,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -5580,7 +5660,7 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -5589,12 +5669,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C4" s="8">
         <f>_measures_details!B29*12*1.005</f>
@@ -5608,7 +5688,7 @@
         <v>4.5454545454545456E-2</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -5623,7 +5703,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -5632,12 +5712,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C5" s="8">
         <v>9200000000</v>
@@ -5649,7 +5729,7 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="G5">
         <v>0.75</v>
@@ -5664,7 +5744,7 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -5687,30 +5767,30 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C53"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -5721,7 +5801,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -5732,7 +5812,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -5743,7 +5823,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -5754,7 +5834,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -5765,7 +5845,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -5776,7 +5856,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -5787,7 +5867,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -5798,7 +5878,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>9</v>
       </c>
@@ -5809,7 +5889,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -5820,7 +5900,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -5831,7 +5911,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12</v>
       </c>
@@ -5842,7 +5922,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -5853,7 +5933,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -5864,7 +5944,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>15</v>
       </c>
@@ -5875,7 +5955,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>16</v>
       </c>
@@ -5886,7 +5966,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>17</v>
       </c>
@@ -5897,7 +5977,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>18</v>
       </c>
@@ -5908,7 +5988,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>19</v>
       </c>
@@ -5919,7 +5999,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>20</v>
       </c>
@@ -5930,7 +6010,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>21</v>
       </c>
@@ -5941,7 +6021,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>22</v>
       </c>
@@ -5952,7 +6032,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>23</v>
       </c>
@@ -5963,7 +6043,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>24</v>
       </c>
@@ -5974,7 +6054,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>25</v>
       </c>
@@ -5985,7 +6065,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>26</v>
       </c>
@@ -5996,7 +6076,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>27</v>
       </c>
@@ -6007,7 +6087,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>28</v>
       </c>
@@ -6018,7 +6098,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>29</v>
       </c>
@@ -6029,7 +6109,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>30</v>
       </c>
@@ -6040,7 +6120,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>31</v>
       </c>
@@ -6051,7 +6131,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>32</v>
       </c>
@@ -6062,7 +6142,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>33</v>
       </c>
@@ -6073,7 +6153,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>34</v>
       </c>
@@ -6084,7 +6164,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>35</v>
       </c>
@@ -6095,7 +6175,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>36</v>
       </c>
@@ -6106,7 +6186,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>37</v>
       </c>
@@ -6117,7 +6197,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>38</v>
       </c>
@@ -6128,7 +6208,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>39</v>
       </c>
@@ -6139,7 +6219,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>40</v>
       </c>
@@ -6150,7 +6230,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>41</v>
       </c>
@@ -6161,7 +6241,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>42</v>
       </c>
@@ -6172,7 +6252,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>43</v>
       </c>
@@ -6183,7 +6263,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>44</v>
       </c>
@@ -6194,7 +6274,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>45</v>
       </c>
@@ -6205,7 +6285,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>46</v>
       </c>
@@ -6216,7 +6296,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>47</v>
       </c>
@@ -6227,7 +6307,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>48</v>
       </c>
@@ -6238,7 +6318,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>49</v>
       </c>
@@ -6249,7 +6329,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>50</v>
       </c>
@@ -6260,7 +6340,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>51</v>
       </c>
@@ -6271,7 +6351,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
       <c r="C53" s="10"/>
     </row>
   </sheetData>
@@ -6286,14 +6366,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" customWidth="1"/>
@@ -6303,26 +6383,26 @@
     <col min="11" max="11" width="15.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="I3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="K3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>2010</v>
       </c>
@@ -6340,7 +6420,7 @@
         <v>657429034020.67725</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2030</v>
       </c>
@@ -6363,7 +6443,7 @@
         <v>670577614701.09082</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="I6">
         <v>2012</v>
       </c>
@@ -6375,7 +6455,7 @@
         <v>683989166995.11267</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="13" thickBot="1">
+    <row r="7" spans="1:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="I7">
         <v>2013</v>
       </c>
@@ -6387,15 +6467,15 @@
         <v>697668950335.01489</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="13" thickBot="1">
+    <row r="8" spans="1:11" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B8" s="26">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="I8">
         <v>2014</v>
@@ -6408,9 +6488,9 @@
         <v>711622329341.71521</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I9">
         <v>2015</v>
@@ -6423,9 +6503,9 @@
         <v>725854775928.54956</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B10" s="11">
         <f>SUM(assets!C2:C51)</f>
@@ -6443,7 +6523,7 @@
         <v>740371871447.12061</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="I11">
         <v>2017</v>
       </c>
@@ -6455,7 +6535,7 @@
         <v>755179308876.06299</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="I12">
         <v>2018</v>
       </c>
@@ -6467,7 +6547,7 @@
         <v>770282895053.58423</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="I13">
         <v>2019</v>
       </c>
@@ -6479,7 +6559,7 @@
         <v>785688552954.65588</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="I14">
         <v>2020</v>
       </c>
@@ -6491,7 +6571,7 @@
         <v>801402324013.74902</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="I15">
         <v>2021</v>
       </c>
@@ -6503,7 +6583,7 @@
         <v>817430370494.02405</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="I16">
         <v>2022</v>
       </c>
@@ -6515,7 +6595,7 @@
         <v>833778977903.90454</v>
       </c>
     </row>
-    <row r="17" spans="9:11">
+    <row r="17" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I17">
         <v>2023</v>
       </c>
@@ -6527,7 +6607,7 @@
         <v>850454557461.98267</v>
       </c>
     </row>
-    <row r="18" spans="9:11">
+    <row r="18" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I18">
         <v>2024</v>
       </c>
@@ -6539,7 +6619,7 @@
         <v>867463648611.22229</v>
       </c>
     </row>
-    <row r="19" spans="9:11">
+    <row r="19" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I19">
         <v>2025</v>
       </c>
@@ -6551,7 +6631,7 @@
         <v>884812921583.44678</v>
       </c>
     </row>
-    <row r="20" spans="9:11">
+    <row r="20" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I20">
         <v>2026</v>
       </c>
@@ -6563,7 +6643,7 @@
         <v>902509180015.11572</v>
       </c>
     </row>
-    <row r="21" spans="9:11">
+    <row r="21" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I21">
         <v>2027</v>
       </c>
@@ -6575,7 +6655,7 @@
         <v>920559363615.41809</v>
       </c>
     </row>
-    <row r="22" spans="9:11">
+    <row r="22" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I22">
         <v>2028</v>
       </c>
@@ -6587,7 +6667,7 @@
         <v>938970550887.72644</v>
       </c>
     </row>
-    <row r="23" spans="9:11">
+    <row r="23" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I23">
         <v>2029</v>
       </c>
@@ -6599,7 +6679,7 @@
         <v>957749961905.48096</v>
       </c>
     </row>
-    <row r="24" spans="9:11">
+    <row r="24" spans="9:11" x14ac:dyDescent="0.15">
       <c r="I24">
         <v>2030</v>
       </c>
@@ -6611,19 +6691,19 @@
         <v>976904961143.59058</v>
       </c>
     </row>
-    <row r="25" spans="9:11">
+    <row r="25" spans="9:11" x14ac:dyDescent="0.15">
       <c r="J25" s="10"/>
     </row>
-    <row r="26" spans="9:11">
+    <row r="26" spans="9:11" x14ac:dyDescent="0.15">
       <c r="J26" s="10"/>
     </row>
-    <row r="27" spans="9:11">
+    <row r="27" spans="9:11" x14ac:dyDescent="0.15">
       <c r="J27" s="10"/>
     </row>
-    <row r="28" spans="9:11">
+    <row r="28" spans="9:11" x14ac:dyDescent="0.15">
       <c r="J28" s="10"/>
     </row>
-    <row r="29" spans="9:11">
+    <row r="29" spans="9:11" x14ac:dyDescent="0.15">
       <c r="J29" s="10"/>
     </row>
   </sheetData>
@@ -6638,14 +6718,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:W29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="23.83203125" customWidth="1"/>
     <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
@@ -6653,14 +6733,14 @@
     <col min="4" max="23" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A2" s="13" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -6675,178 +6755,178 @@
       <c r="L2" s="13"/>
       <c r="M2" s="13"/>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23">
-      <c r="A6" t="s">
-        <v>25</v>
       </c>
       <c r="B6" s="10">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B7" s="10">
         <v>0.2</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B8" s="20">
         <f>B6*SUM(assets!C2:C51)*_measures_details!B7</f>
         <v>131410658911.98209</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B11" s="11">
         <v>4000000</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B12" s="20">
         <f>_discounting_sheet!D4</f>
         <v>69405733.37838845</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.15">
       <c r="W13" s="14" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B16" s="11">
         <v>20000000</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B17" s="11">
         <v>500000</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B18" s="11">
         <v>500000</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B19" s="11">
         <v>400000</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B20" s="20">
         <f>_discounting_sheet!F4</f>
         <v>43892006.68243596</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B24">
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B25" s="11">
         <v>30000</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B26" s="14">
         <f>B24^2*B25*2000</f>
         <v>540000000</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B27">
         <v>400</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B28" s="14">
         <f>B25*B27</f>
         <v>12000000</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B29" s="20">
         <f>_discounting_sheet!H4</f>
@@ -6866,14 +6946,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
@@ -6884,39 +6964,39 @@
     <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="M3" s="16"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>2010</v>
       </c>
@@ -6952,7 +7032,7 @@
       <c r="L4" s="16"/>
       <c r="M4" s="18"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2011</v>
       </c>
@@ -6988,7 +7068,7 @@
       <c r="L5" s="16"/>
       <c r="M5" s="15"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>2012</v>
       </c>
@@ -7024,7 +7104,7 @@
       <c r="L6" s="16"/>
       <c r="M6" s="15"/>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>2013</v>
       </c>
@@ -7060,7 +7140,7 @@
       <c r="L7" s="16"/>
       <c r="M7" s="15"/>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>2014</v>
       </c>
@@ -7096,7 +7176,7 @@
       <c r="L8" s="16"/>
       <c r="M8" s="15"/>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>2015</v>
       </c>
@@ -7132,7 +7212,7 @@
       <c r="L9" s="16"/>
       <c r="M9" s="15"/>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>2016</v>
       </c>
@@ -7168,7 +7248,7 @@
       <c r="L10" s="16"/>
       <c r="M10" s="15"/>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>2017</v>
       </c>
@@ -7204,7 +7284,7 @@
       <c r="L11" s="16"/>
       <c r="M11" s="15"/>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>2018</v>
       </c>
@@ -7240,7 +7320,7 @@
       <c r="L12" s="16"/>
       <c r="M12" s="15"/>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>2019</v>
       </c>
@@ -7276,7 +7356,7 @@
       <c r="L13" s="16"/>
       <c r="M13" s="15"/>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>2020</v>
       </c>
@@ -7312,7 +7392,7 @@
       <c r="L14" s="16"/>
       <c r="M14" s="15"/>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -7348,7 +7428,7 @@
       <c r="L15" s="16"/>
       <c r="M15" s="15"/>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>2022</v>
       </c>
@@ -7384,7 +7464,7 @@
       <c r="L16" s="16"/>
       <c r="M16" s="15"/>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>2023</v>
       </c>
@@ -7420,7 +7500,7 @@
       <c r="L17" s="16"/>
       <c r="M17" s="15"/>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>2024</v>
       </c>
@@ -7456,7 +7536,7 @@
       <c r="L18" s="16"/>
       <c r="M18" s="15"/>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>2025</v>
       </c>
@@ -7492,7 +7572,7 @@
       <c r="L19" s="16"/>
       <c r="M19" s="15"/>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>2026</v>
       </c>
@@ -7528,7 +7608,7 @@
       <c r="L20" s="16"/>
       <c r="M20" s="15"/>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>2027</v>
       </c>
@@ -7564,7 +7644,7 @@
       <c r="L21" s="16"/>
       <c r="M21" s="15"/>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>2028</v>
       </c>
@@ -7600,7 +7680,7 @@
       <c r="L22" s="16"/>
       <c r="M22" s="15"/>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>2029</v>
       </c>
@@ -7636,7 +7716,7 @@
       <c r="L23" s="16"/>
       <c r="M23" s="15"/>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>2030</v>
       </c>

</xml_diff>